<commit_message>
Compiled CSD fitting results
</commit_message>
<xml_diff>
--- a/fitters/cluster_size_distribution.xlsx
+++ b/fitters/cluster_size_distribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Github\vegetation-dynamics\fitters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC863E3E-CBE0-476E-9E3F-5E24FFE4D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA03C35-A136-483C-8D32-AB7CE2A5F84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>p</t>
   </si>
@@ -42,9 +42,6 @@
     <t>0p616</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>0p618</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>0p7</t>
   </si>
   <si>
-    <t>0p72</t>
-  </si>
-  <si>
     <t>q = 0</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>0p53</t>
   </si>
   <si>
-    <t>0p55</t>
-  </si>
-  <si>
     <t>0p399</t>
   </si>
   <si>
@@ -147,7 +138,37 @@
     <t>0p41</t>
   </si>
   <si>
-    <t>0p42</t>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>0p73</t>
+  </si>
+  <si>
+    <t>0p74</t>
+  </si>
+  <si>
+    <t>0p66</t>
+  </si>
+  <si>
+    <t>0p72 (P)</t>
+  </si>
+  <si>
+    <t>0p56</t>
+  </si>
+  <si>
+    <t>0p43</t>
+  </si>
+  <si>
+    <t>0p44</t>
+  </si>
+  <si>
+    <t>0p64 (P)</t>
+  </si>
+  <si>
+    <t>0p55 (P)</t>
+  </si>
+  <si>
+    <t>0p42 (P)</t>
   </si>
 </sst>
 </file>
@@ -163,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,12 +194,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,11 +216,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,39 +503,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T13"/>
+  <dimension ref="B2:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="L2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="Q2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="Q2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -577,428 +591,528 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
+      <c r="C4">
+        <v>4425.2016246515504</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4157.8117020005802</v>
+      </c>
+      <c r="E4">
+        <v>4187.1850761953101</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>30168.830556783199</v>
+      </c>
+      <c r="I4" s="1">
+        <v>28825.167373437798</v>
+      </c>
+      <c r="J4">
+        <v>29852.174985378799</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="M4">
+        <v>33174.865489999996</v>
+      </c>
+      <c r="N4">
+        <v>32135.811679999999</v>
+      </c>
+      <c r="O4">
+        <v>34534.79333</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T4" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="R4">
+        <v>21254.602080000001</v>
+      </c>
+      <c r="S4" s="1">
+        <v>20857.27778</v>
+      </c>
+      <c r="T4">
+        <v>24082.582060000001</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
+      <c r="C5">
+        <v>11973.852875651501</v>
+      </c>
+      <c r="D5" s="1">
+        <v>11304.233324840699</v>
+      </c>
+      <c r="E5">
+        <v>11476.2547304584</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>682.98736689999998</v>
+        <v>75647.203866649899</v>
       </c>
       <c r="I5" s="1">
-        <v>663.78861649999999</v>
+        <v>72401.878107224504</v>
       </c>
       <c r="J5">
-        <v>678.92406919999996</v>
+        <v>75340.037837104406</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M5">
-        <v>607.05897779999998</v>
+        <v>67667.954209999996</v>
       </c>
       <c r="N5" s="1">
-        <v>595.35353620000001</v>
+        <v>65470.872949999997</v>
       </c>
       <c r="O5">
-        <v>630.86402120000002</v>
+        <v>70297.171759999997</v>
       </c>
       <c r="Q5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" t="s">
-        <v>5</v>
-      </c>
-      <c r="S5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T5" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="R5">
+        <v>31567.658329999998</v>
+      </c>
+      <c r="S5" s="1">
+        <v>30960.296330000001</v>
+      </c>
+      <c r="T5">
+        <v>35739.93316</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>27887.9501979706</v>
+      </c>
+      <c r="D6" s="1">
+        <v>26370.7072239804</v>
+      </c>
+      <c r="E6">
+        <v>26864.0666757217</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H6">
-        <v>812.89021849999995</v>
+        <v>90301.041002949205</v>
       </c>
       <c r="I6" s="1">
-        <v>788.56386659999998</v>
+        <v>86394.570573662699</v>
       </c>
       <c r="J6">
-        <v>808.68818959999999</v>
+        <v>89926.119110094704</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M6">
-        <v>969.12728960000004</v>
+        <v>108497.8873</v>
       </c>
       <c r="N6" s="1">
-        <v>948.6469525</v>
+        <v>105264.8624</v>
       </c>
       <c r="O6">
-        <v>1019.311914</v>
+        <v>114229.8876</v>
       </c>
       <c r="Q6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="1">
-        <v>464.48469563716299</v>
-      </c>
-      <c r="S6">
-        <v>467.19949455706302</v>
+        <v>33</v>
+      </c>
+      <c r="R6" s="2">
+        <v>52055.197670000001</v>
+      </c>
+      <c r="S6" s="1">
+        <v>51048.237990000001</v>
       </c>
       <c r="T6">
-        <v>524.32001308728002</v>
+        <v>58973.353880000002</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>886.14403470000002</v>
+        <v>98231.876875185495</v>
       </c>
       <c r="D7" s="1">
-        <v>841.8202106</v>
+        <v>92871.539674619897</v>
       </c>
       <c r="E7">
-        <v>855.25691979999999</v>
+        <v>94805.809566260694</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H7">
-        <v>1486.6239929999999</v>
+        <v>166538.28998396001</v>
       </c>
       <c r="I7" s="1">
-        <v>1434.4738150000001</v>
+        <v>160154.56013777401</v>
       </c>
       <c r="J7">
-        <v>1505.7790709999999</v>
+        <v>168700.16392681599</v>
       </c>
       <c r="L7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M7">
-        <v>1272.2885879999999</v>
+        <v>142998.36900000001</v>
       </c>
       <c r="N7" s="1">
-        <v>1255.391265</v>
+        <v>138946.0336</v>
       </c>
       <c r="O7">
-        <v>1352.1670429999999</v>
+        <v>151953.41029999999</v>
       </c>
       <c r="Q7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="2">
+        <v>92475.80025</v>
+      </c>
+      <c r="S7" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="1">
-        <v>812.86130493563201</v>
-      </c>
-      <c r="S7">
-        <v>813.43139120215801</v>
-      </c>
       <c r="T7">
-        <v>970.58688150702994</v>
+        <v>110282.5831</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>1538.9778080000001</v>
+        <v>171619.19560840001</v>
       </c>
       <c r="D8" s="1">
-        <v>1468.189599</v>
+        <v>162872.88513594199</v>
       </c>
       <c r="E8">
-        <v>1500.6510760000001</v>
+        <v>167262.263410154</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H8">
-        <v>1954.3233310000001</v>
+        <v>220242.05004832501</v>
       </c>
       <c r="I8" s="1">
-        <v>1897.895571</v>
+        <v>212369.577889081</v>
       </c>
       <c r="J8">
-        <v>2008.6968449999999</v>
+        <v>225939.285125147</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M8">
-        <v>1505.20857</v>
+        <v>169914.5374</v>
       </c>
       <c r="N8" s="1">
-        <v>1477.8634179999999</v>
+        <v>165439.25330000001</v>
       </c>
       <c r="O8">
-        <v>1618.7433860000001</v>
+        <v>182482.2427</v>
       </c>
       <c r="Q8" t="s">
-        <v>38</v>
-      </c>
-      <c r="R8" s="1">
-        <v>1081.3095454115601</v>
-      </c>
-      <c r="S8">
-        <v>1097.0997712180799</v>
+        <v>35</v>
+      </c>
+      <c r="R8" s="2">
+        <v>125717.2552</v>
+      </c>
+      <c r="S8" s="1">
+        <v>124330.3918</v>
       </c>
       <c r="T8">
-        <v>1347.5713441841899</v>
+        <v>154985.67060000001</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>253490.427179552</v>
+      </c>
+      <c r="D9" s="1">
+        <v>242703.145671648</v>
+      </c>
+      <c r="E9">
+        <v>253484.53806836301</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>270730.37758025399</v>
+      </c>
+      <c r="I9" s="1">
+        <v>263229.15382493701</v>
+      </c>
+      <c r="J9">
+        <v>288691.03733550297</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9">
+        <v>189161.204</v>
+      </c>
+      <c r="N9" s="1">
+        <v>184697.45069999999</v>
+      </c>
+      <c r="O9">
+        <v>206568.03880000001</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="2">
+        <v>142780.90700000001</v>
+      </c>
+      <c r="S9" s="1">
+        <v>142112.64060000001</v>
+      </c>
+      <c r="T9">
+        <v>198161.21350000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
-        <v>2257.6755720000001</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2173.6664449999998</v>
-      </c>
-      <c r="E9">
-        <v>2261.070886</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9">
-        <v>2379.2114809999998</v>
-      </c>
-      <c r="I9" s="1">
-        <v>2325.0311609999999</v>
-      </c>
-      <c r="J9">
-        <v>2549.7320319999999</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="C10">
+        <v>296095.38154216303</v>
+      </c>
+      <c r="D10" s="1">
+        <v>285197.438170515</v>
+      </c>
+      <c r="E10">
+        <v>302917.64475005999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>240271.55089452301</v>
+      </c>
+      <c r="I10" s="1">
+        <v>237755.908253945</v>
+      </c>
+      <c r="J10">
+        <v>298303.032985995</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10">
+        <v>204701.44870000001</v>
+      </c>
+      <c r="N10" s="1">
+        <v>200164.4387</v>
+      </c>
+      <c r="O10">
+        <v>225851.47700000001</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>47</v>
+      </c>
+      <c r="R10" s="2">
+        <v>98499.346950000006</v>
+      </c>
+      <c r="S10" s="1">
+        <v>98497.334340000001</v>
+      </c>
+      <c r="T10">
+        <v>176588.399</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>234874.094764212</v>
+      </c>
+      <c r="D11" s="1">
+        <v>232769.863606005</v>
+      </c>
+      <c r="E11">
+        <v>298873.79634435801</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <v>166263.874054935</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11">
+        <v>247462.47188441199</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M9">
-        <v>1666.500329</v>
-      </c>
-      <c r="N9" s="1">
-        <v>1638.9988530000001</v>
-      </c>
-      <c r="O9">
-        <v>1826.836135</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="M11">
+        <v>225949.55410000001</v>
+      </c>
+      <c r="N11" s="1">
+        <v>222869.34669999999</v>
+      </c>
+      <c r="O11">
+        <v>268707.82490000001</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="1">
+        <v>58810.288</v>
+      </c>
+      <c r="S11">
+        <v>58823.034460000003</v>
+      </c>
+      <c r="T11">
+        <v>139618.02799999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12">
+        <v>151712.514620239</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>237533.64575078301</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>123673.382216714</v>
+      </c>
+      <c r="I12" s="1">
+        <v>123666.719871689</v>
+      </c>
+      <c r="J12">
+        <v>213953.069201971</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12">
+        <v>205542.12419999999</v>
+      </c>
+      <c r="N12" s="1">
+        <v>204648.38130000001</v>
+      </c>
+      <c r="O12">
+        <v>266147.0626</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="1">
+        <v>38191.124629999998</v>
+      </c>
+      <c r="S12">
+        <v>38207.059459999997</v>
+      </c>
+      <c r="T12">
+        <v>110325.0512</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>114450.29366386701</v>
+      </c>
+      <c r="D13" s="1">
+        <v>114446.38916084501</v>
+      </c>
+      <c r="E13">
+        <v>204507.027477631</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="1">
+        <v>91820.213602750198</v>
+      </c>
+      <c r="I13">
+        <v>91826.837693075402</v>
+      </c>
+      <c r="J13">
+        <v>186302.145345261</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="2">
+        <v>126758.89840000001</v>
+      </c>
+      <c r="N13" s="1">
+        <v>126748.87300000001</v>
+      </c>
+      <c r="O13">
+        <v>212344.5736</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="1">
-        <v>1175.4079565167101</v>
-      </c>
-      <c r="S9">
-        <v>1158.1435922641599</v>
-      </c>
-      <c r="T9">
-        <v>1686.6955948017901</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
-        <v>2621.6308859999999</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2537.7204620000002</v>
-      </c>
-      <c r="E10" s="3">
-        <v>2688.9054700000002</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2003.762954</v>
-      </c>
-      <c r="I10">
-        <v>2013.7094790000001</v>
-      </c>
-      <c r="J10">
-        <v>2558.6583089999999</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10">
-        <v>1795.3317790000001</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1767.6098509999999</v>
-      </c>
-      <c r="O10">
-        <v>1989.477705</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>40</v>
-      </c>
-      <c r="R10" s="1">
-        <v>718.00084414419905</v>
-      </c>
-      <c r="S10">
-        <v>726.45208820366804</v>
-      </c>
-      <c r="T10">
-        <v>1444.5023772883001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1933.096358</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1947.3203000000001</v>
-      </c>
-      <c r="E11" s="3">
-        <v>2540.3215500000001</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1283.0510670000001</v>
-      </c>
-      <c r="I11">
-        <v>1280.465142</v>
-      </c>
-      <c r="J11">
-        <v>2056.6217809999998</v>
-      </c>
-      <c r="L11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11">
-        <v>1942.5975880000001</v>
-      </c>
-      <c r="N11" s="1">
-        <v>1936.8469259999999</v>
-      </c>
-      <c r="O11">
-        <v>2337.9051570000001</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1126.969591</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1137.580087</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1952.4114939999999</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M12">
-        <v>1711.5320139999999</v>
-      </c>
-      <c r="N12" s="1">
-        <v>1728.973463</v>
-      </c>
-      <c r="O12">
-        <v>2277.5638560000002</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="L13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" s="1">
-        <v>928.64912570000001</v>
-      </c>
-      <c r="N13">
-        <v>937.5424342</v>
-      </c>
-      <c r="O13">
-        <v>1744.514741</v>
+      <c r="C14" s="1">
+        <v>82079.274526811001</v>
+      </c>
+      <c r="D14">
+        <v>82087.995842854798</v>
+      </c>
+      <c r="E14">
+        <v>174193.41604815601</v>
+      </c>
+      <c r="L14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14">
+        <v>89945.423729999995</v>
+      </c>
+      <c r="N14" t="s">
+        <v>37</v>
+      </c>
+      <c r="O14">
+        <v>181368.17809999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="L15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="1">
+        <v>63808.336640000001</v>
+      </c>
+      <c r="N15">
+        <v>63821.59345</v>
+      </c>
+      <c r="O15">
+        <v>153021.93659999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>